<commit_message>
Update olfactory conditioning tests
</commit_message>
<xml_diff>
--- a/src/incentive/data/bennett2021/41467_2021_22592_MOESM4_ESM.xlsx
+++ b/src/incentive/data/bennett2021/41467_2021_22592_MOESM4_ESM.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Testing time (miutes after training)</t>
   </si>
   <si>
-    <t xml:space="preserve">Cell model</t>
+    <t xml:space="preserve">Plausible model</t>
   </si>
   <si>
     <t xml:space="preserve">Cell types</t>
@@ -195,378 +195,381 @@
     <t xml:space="preserve">5B</t>
   </si>
   <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012burke.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burke et al. (2012), Layered reward signalling through octopamine and dopamine in Drosophila, Nature 492, 433-437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012liu.tanimoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liu et al. (2012), A subset of dopamine neurons signals reward for odour memory in Drosophila, Nature 488, 512-516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013placais.preat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placais et al. (2013), Two pairs of mushroom body efferent neurons are required for appetitive long-term memory retrieval in Drosophila, Cell Reports 5, 769-780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014aso.rubin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aso et al. (2014), Mushroom body output neurons encode valence and guide memory-based action selection in Drosophila, eLife 3:e04580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014lin.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lin et al. (2014), Neural correlates of water reward in thirsty Drosophila, Nature Neuroscience 17, 1536-1542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015huetteroth.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huetteroth et al. (2015), Sweet taste and nutrient value subdivide rewarding dopaminergic neurons in Drosophila, Current Biology 25, 751-758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F,3I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ichinose et al. (2015), Reward signal in a recurrent circuit drives appetitive long-term memory formation, eLife 4:e10719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015owald.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owald et al. (2015), Activity of defined mushroom body output neurons underlies learned olfactory behaviour in Drosophila, Neuron 86, 417-427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM Y4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016aso.rubin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aso &amp; Rubin (2016), Dopaminergic neurons write and update memories with cell-type-specific rules, eLife 5:e16135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM inc. any of a1, B1, B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016perisse.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perisse et al. (2016), Aversive learning and appetitive motivation toggle feed-forward inhibition in the Drosophila mushroom body, Neuron 90, 1086-1099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B, 3C, 3D, 3E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM a1, or B1B2, or Y5B'2 (60s odour + 30x1s light) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016yamagata.tanimoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yamagata et al. (2016), Supression of dopamine neurons mediates reward, PLoS Biology 14, e1002586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017felsenberg.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felsenberg et al. (2017), Re-evaluation of learned information in Drosophila, Nature 544, 240-244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM a1, or B1B2 (10s odour + 3x1s light)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4B, 4D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM Y3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 cluster + DAN PAM B2B'2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 Y1-pedc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 a2a'2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM B1B'2 (supposedly aversive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B, 2C, 3C, 3D, 3E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1, a3 (60s odour + 30x1s light)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1 (60s odour + 30x1s light)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1 (10s odour + 3x1s light)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1, a3 (60s odour + 30x1s light, repeated 10 times)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON MB-V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM, multiple drivers that label at least Y5b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PAM a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A, 5B (right column)</t>
+  </si>
+  <si>
     <t xml:space="preserve">r</t>
   </si>
   <si>
-    <t xml:space="preserve">MBON a1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012burke.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burke et al. (2012), Layered reward signalling through octopamine and dopamine in Drosophila, Nature 492, 433-437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012liu.tanimoto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liu et al. (2012), A subset of dopamine neurons signals reward for odour memory in Drosophila, Nature 488, 512-516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013placais.preat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placais et al. (2013), Two pairs of mushroom body efferent neurons are required for appetitive long-term memory retrieval in Drosophila, Cell Reports 5, 769-780</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014aso.rubin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aso et al. (2014), Mushroom body output neurons encode valence and guide memory-based action selection in Drosophila, eLife 3:e04580</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014lin.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lin et al. (2014), Neural correlates of water reward in thirsty Drosophila, Nature Neuroscience 17, 1536-1542</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015huetteroth.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huetteroth et al. (2015), Sweet taste and nutrient value subdivide rewarding dopaminergic neurons in Drosophila, Current Biology 25, 751-758</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3F,3I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM cluster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ichinose et al. (2015), Reward signal in a recurrent circuit drives appetitive long-term memory formation, eLife 4:e10719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015owald.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owald et al. (2015), Activity of defined mushroom body output neurons underlies learned olfactory behaviour in Drosophila, Neuron 86, 417-427</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM Y4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016aso.rubin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aso &amp; Rubin (2016), Dopaminergic neurons write and update memories with cell-type-specific rules, eLife 5:e16135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dcf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM inc. any of a1, B1, B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016perisse.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perisse et al. (2016), Aversive learning and appetitive motivation toggle feed-forward inhibition in the Drosophila mushroom body, Neuron 90, 1086-1099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2B, 3C, 3D, 3E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM a1, or B1B2, or Y5B'2 (60s odour + 30x1s light) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016yamagata.tanimoto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yamagata et al. (2016), Supression of dopamine neurons mediates reward, PLoS Biology 14, e1002586</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017felsenberg.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Felsenberg et al. (2017), Re-evaluation of learned information in Drosophila, Nature 544, 240-244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM a1, or B1B2 (10s odour + 3x1s light)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4B, 4D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM Y3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 cluster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 cluster + DAN PAM B2B'2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 Y1-pedc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 a2a'2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM B1B'2 (supposedly aversive)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2B, 2C, 3C, 3D, 3E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1, a3 (60s odour + 30x1s light)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1 (60s odour + 30x1s light)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1 (10s odour + 3x1s light)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 Y1-pedc, a'2a2 + Y2a'1, a3 (60s odour + 30x1s light, repeated 10 times)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON MB-V3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3H</t>
+    <t xml:space="preserve">MBON MB-V3, inc. ChAT RNAi knockdown of Ach, 5 x spaced training trials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A, 5B (middle column)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON MB-V3, inc. ChAT RNAi knockdown of Ach, 5 x massed training trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A, 5B (left column)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON MB-V3, inc. ChAT RNAi knockdown of Ach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON Y1-pedc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2H</t>
   </si>
   <si>
     <t xml:space="preserve">sm</t>
   </si>
   <si>
-    <t xml:space="preserve">2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM, multiple drivers that label at least Y5b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PAM a1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5A, 5B (right column)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON MB-V3, inc. ChAT RNAi knockdown of Ach, 5 x spaced training trials </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5A, 5B (middle column)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON MB-V3, inc. ChAT RNAi knockdown of Ach, 5 x massed training trials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5A, 5B (left column)</t>
+    <t xml:space="preserve">2E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON MB-V2 (a2sc + a'1 + a2p3p + a'3ap + a'3m)</t>
   </si>
   <si>
     <t xml:space="preserve">rm</t>
   </si>
   <si>
-    <t xml:space="preserve">MBON MB-V3, inc. ChAT RNAi knockdown of Ach </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y1-pedc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6B</t>
+    <t xml:space="preserve">MBON Y2a'1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013placais.waddell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON MB-V3, 5 x spaced training trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON Y1-pedc (food sated before testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON Y1-pedc (starved before testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON B'2mp, Y5B'2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON B2B'2a, B'2mp, Y5B'2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON Y5B'2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2E, 4F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplementary 5G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 y1-pedc (food sated before testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplementary 5H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 y1-pedc (starved before testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN PPL1 Y2a'1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6B, 6C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON Y1-pedc (olfactory, two different drivers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8B, 8C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON Y1-pedc (visual, two different drivers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON a3 + a'2, a'2 + Y2a'1, Y2a'1, a2a3 + a'3 + a'1, a'3, a2 + a2a3 + a'3 + a'1 (visual)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBON a1, a'2 , a2 + a3 + a'3 + a'1 (olfactory)</t>
   </si>
   <si>
     <t xml:space="preserve">srm</t>
   </si>
   <si>
-    <t xml:space="preserve">6C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON MB-V2 (a2sc + a'1 + a2p3p + a'3ap + a'3m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y2a'1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013placais.waddell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON MB-V3, 5 x spaced training trials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y1-pedc (food sated before testing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y1-pedc (starved before testing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON B'2mp, Y5B'2a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON B2B'2a, B'2mp, Y5B'2a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y5B'2a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2E, 4F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplementary 5G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 y1-pedc (food sated before testing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplementary 5H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 y1-pedc (starved before testing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAN PPL1 Y2a'1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6B, 6C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y1-pedc (olfactory, two different drivers)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8B, 8C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON Y1-pedc (visual, two different drivers)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON a3 + a'2, a'2 + Y2a'1, Y2a'1, a2a3 + a'3 + a'1, a'3, a2 + a2a3 + a'3 + a'1 (visual)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBON a1, a'2 , a2 + a3 + a'3 + a'1 (olfactory)</t>
-  </si>
-  <si>
     <t xml:space="preserve">MBON MB-V3: RNAi experiment to knockdown Ach transmission in MB-V3.</t>
   </si>
   <si>
@@ -619,9 +622,6 @@
   </si>
   <si>
     <t xml:space="preserve">2C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df</t>
   </si>
   <si>
     <t xml:space="preserve">2N</t>
@@ -773,7 +773,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -846,6 +846,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right/>
       <top style="thin"/>
       <bottom/>
@@ -884,7 +891,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1237,6 +1244,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1341,7 +1352,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1357,7 +1368,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1469,14 +1480,14 @@
   <dimension ref="A1:AS171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AH89" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AF1" activeCellId="0" sqref="AF1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI163" activeCellId="0" sqref="AI163"/>
+      <selection pane="topRight" activeCell="AH1" activeCellId="0" sqref="AH1"/>
+      <selection pane="bottomLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="AI1" activeCellId="0" sqref="AI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.33"/>
@@ -1499,7 +1510,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="43.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="34.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="25.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="39.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="33.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="11.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="63.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="50.86"/>
@@ -3103,16 +3114,16 @@
         <v>2</v>
       </c>
       <c r="AI21" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AJ21" s="65" t="s">
         <v>60</v>
       </c>
       <c r="AK21" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL21" s="40" t="s">
         <v>64</v>
-      </c>
-      <c r="AL21" s="40" t="s">
-        <v>65</v>
       </c>
       <c r="AM21" s="40"/>
       <c r="AN21" s="40"/>
@@ -3190,22 +3201,22 @@
         <v>54</v>
       </c>
       <c r="AG22" s="63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AH22" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI22" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AJ22" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK22" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="AK22" s="39" t="s">
+      <c r="AL22" s="40" t="s">
         <v>68</v>
-      </c>
-      <c r="AL22" s="40" t="s">
-        <v>69</v>
       </c>
       <c r="AM22" s="40"/>
       <c r="AN22" s="40"/>
@@ -3313,22 +3324,22 @@
         <v>56</v>
       </c>
       <c r="AG23" s="63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AH23" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI23" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ23" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="AJ23" s="65" t="s">
+      <c r="AK23" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="AK23" s="39" t="s">
+      <c r="AL23" s="40" t="s">
         <v>73</v>
-      </c>
-      <c r="AL23" s="40" t="s">
-        <v>74</v>
       </c>
       <c r="AM23" s="40"/>
       <c r="AN23" s="40"/>
@@ -3423,25 +3434,25 @@
         <v>1.96609956292897</v>
       </c>
       <c r="AF24" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG24" s="63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AH24" s="64" t="n">
         <v>1</v>
       </c>
       <c r="AI24" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AJ24" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK24" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK24" s="39" t="s">
+      <c r="AL24" s="40" t="s">
         <v>77</v>
-      </c>
-      <c r="AL24" s="40" t="s">
-        <v>78</v>
       </c>
       <c r="AM24" s="40"/>
       <c r="AN24" s="40"/>
@@ -3518,25 +3529,25 @@
         <v>0.802572353905128</v>
       </c>
       <c r="AF25" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG25" s="63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH25" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI25" s="64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AJ25" s="65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AK25" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL25" s="40" t="s">
         <v>80</v>
-      </c>
-      <c r="AL25" s="40" t="s">
-        <v>81</v>
       </c>
       <c r="AM25" s="40"/>
       <c r="AN25" s="40"/>
@@ -3613,16 +3624,16 @@
         <v>0.869939932464054</v>
       </c>
       <c r="AF26" s="70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG26" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH26" s="72" t="n">
         <v>1</v>
       </c>
       <c r="AI26" s="72" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="AJ26" s="73" t="s">
         <v>83</v>
@@ -3838,7 +3849,7 @@
         <v>1.27500398439368</v>
       </c>
       <c r="AF29" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG29" s="25" t="s">
         <v>84</v>
@@ -4054,15 +4065,13 @@
       <c r="AH32" s="64" t="n">
         <v>7</v>
       </c>
-      <c r="AI32" s="64" t="s">
-        <v>85</v>
-      </c>
+      <c r="AI32" s="64"/>
       <c r="AJ32" s="82" t="s">
         <v>89</v>
       </c>
       <c r="AK32" s="83"/>
     </row>
-    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4142,7 +4151,7 @@
         <v>2</v>
       </c>
       <c r="AI33" s="64" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="AJ33" s="65" t="s">
         <v>91</v>
@@ -4234,7 +4243,7 @@
       </c>
       <c r="AK34" s="83"/>
     </row>
-    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4308,14 +4317,14 @@
         <v>2</v>
       </c>
       <c r="AI35" s="64" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AJ35" s="65" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK35" s="83"/>
     </row>
-    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4383,20 +4392,20 @@
         <v>40</v>
       </c>
       <c r="AG36" s="63" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AH36" s="64" t="n">
         <v>2</v>
       </c>
       <c r="AI36" s="64" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="AJ36" s="65" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK36" s="83"/>
     </row>
-    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4472,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="AI37" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AJ37" s="65" t="s">
         <v>60</v>
@@ -4547,7 +4556,7 @@
         <v>52</v>
       </c>
       <c r="AG38" s="63" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AH38" s="64" t="n">
         <v>3</v>
@@ -4560,7 +4569,7 @@
       </c>
       <c r="AK38" s="83"/>
     </row>
-    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4643,10 +4652,10 @@
         <v>2.23079016664105</v>
       </c>
       <c r="AF39" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG39" s="63" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AH39" s="64" t="n">
         <v>1</v>
@@ -4655,11 +4664,11 @@
         <v>93</v>
       </c>
       <c r="AJ39" s="65" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK39" s="83"/>
     </row>
-    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4724,10 +4733,10 @@
         <v>0.525725014711065</v>
       </c>
       <c r="AF40" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG40" s="63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH40" s="64" t="n">
         <v>1440</v>
@@ -4736,11 +4745,11 @@
         <v>93</v>
       </c>
       <c r="AJ40" s="65" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AK40" s="83"/>
     </row>
-    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="57" t="n">
         <v>1423</v>
       </c>
@@ -4805,19 +4814,19 @@
         <v>1.56896173413483</v>
       </c>
       <c r="AF41" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG41" s="63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH41" s="64" t="n">
         <v>1</v>
       </c>
       <c r="AI41" s="64" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="AJ41" s="65" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AK41" s="83"/>
     </row>
@@ -4888,19 +4897,19 @@
         <v>1.39676218585035</v>
       </c>
       <c r="AF42" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG42" s="63" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AH42" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI42" s="64" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="AJ42" s="65" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AK42" s="83"/>
     </row>
@@ -4971,23 +4980,23 @@
         <v>0.819403721760565</v>
       </c>
       <c r="AF43" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG43" s="63" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AH43" s="64" t="n">
         <v>5760</v>
       </c>
       <c r="AI43" s="64" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="AJ43" s="65" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AK43" s="83"/>
     </row>
-    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="19" t="n">
         <v>1423</v>
       </c>
@@ -5056,22 +5065,24 @@
         <v>-1.61346108034111</v>
       </c>
       <c r="AF44" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG44" s="71" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AH44" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="AI44" s="72"/>
+      <c r="AI44" s="88" t="s">
+        <v>59</v>
+      </c>
       <c r="AJ44" s="73" t="s">
         <v>86</v>
       </c>
       <c r="AK44" s="83"/>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="88" t="n">
+      <c r="A45" s="89" t="n">
         <v>2111</v>
       </c>
       <c r="B45" s="76"/>
@@ -5136,37 +5147,37 @@
       <c r="AK45" s="35"/>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="89" t="n">
+      <c r="A46" s="90" t="n">
         <v>2112</v>
       </c>
-      <c r="B46" s="90" t="n">
+      <c r="B46" s="91" t="n">
         <v>0.31</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
-      <c r="M46" s="90"/>
-      <c r="N46" s="91" t="n">
+      <c r="C46" s="91"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="91"/>
+      <c r="F46" s="91"/>
+      <c r="G46" s="91"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="91"/>
+      <c r="N46" s="92" t="n">
         <v>0.35</v>
       </c>
-      <c r="O46" s="91" t="n">
+      <c r="O46" s="92" t="n">
         <v>0.37</v>
       </c>
-      <c r="P46" s="91"/>
-      <c r="Q46" s="91"/>
-      <c r="R46" s="91"/>
-      <c r="S46" s="91"/>
-      <c r="T46" s="91"/>
-      <c r="U46" s="91"/>
-      <c r="V46" s="91"/>
-      <c r="W46" s="91"/>
+      <c r="P46" s="92"/>
+      <c r="Q46" s="92"/>
+      <c r="R46" s="92"/>
+      <c r="S46" s="92"/>
+      <c r="T46" s="92"/>
+      <c r="U46" s="92"/>
+      <c r="V46" s="92"/>
+      <c r="W46" s="92"/>
       <c r="X46" s="22" t="n">
         <f aca="false">AVERAGE(B46:M46)</f>
         <v>0.31</v>
@@ -5202,22 +5213,22 @@
       <c r="AF46" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="AG46" s="92" t="s">
-        <v>104</v>
+      <c r="AG46" s="93" t="s">
+        <v>106</v>
       </c>
       <c r="AH46" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI46" s="64" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AJ46" s="82" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK46" s="83"/>
     </row>
     <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="89" t="n">
+      <c r="A47" s="90" t="n">
         <v>2113</v>
       </c>
       <c r="B47" s="20"/>
@@ -5282,7 +5293,7 @@
       <c r="AK47" s="35"/>
     </row>
     <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="89" t="n">
+      <c r="A48" s="90" t="n">
         <v>2121</v>
       </c>
       <c r="B48" s="20"/>
@@ -5347,7 +5358,7 @@
       <c r="AK48" s="35"/>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="89" t="n">
+      <c r="A49" s="90" t="n">
         <v>2122</v>
       </c>
       <c r="B49" s="20"/>
@@ -5412,7 +5423,7 @@
       <c r="AK49" s="35"/>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="89" t="n">
+      <c r="A50" s="90" t="n">
         <v>2123</v>
       </c>
       <c r="B50" s="20"/>
@@ -5477,7 +5488,7 @@
       <c r="AK50" s="35"/>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="89" t="n">
+      <c r="A51" s="90" t="n">
         <v>2211</v>
       </c>
       <c r="B51" s="20"/>
@@ -5542,7 +5553,7 @@
       <c r="AK51" s="35"/>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="89" t="n">
+      <c r="A52" s="90" t="n">
         <v>2212</v>
       </c>
       <c r="B52" s="20" t="n">
@@ -5613,13 +5624,13 @@
         <v>42</v>
       </c>
       <c r="AG52" s="25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AH52" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI52" s="64" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AJ52" s="27" t="s">
         <v>45</v>
@@ -5627,7 +5638,7 @@
       <c r="AK52" s="35"/>
     </row>
     <row r="53" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="89" t="n">
+      <c r="A53" s="90" t="n">
         <v>2213</v>
       </c>
       <c r="B53" s="20"/>
@@ -5692,7 +5703,7 @@
       <c r="AK53" s="35"/>
     </row>
     <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="89" t="n">
+      <c r="A54" s="90" t="n">
         <v>2221</v>
       </c>
       <c r="B54" s="20"/>
@@ -5757,7 +5768,7 @@
       <c r="AK54" s="35"/>
     </row>
     <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="89" t="n">
+      <c r="A55" s="90" t="n">
         <v>2222</v>
       </c>
       <c r="B55" s="20"/>
@@ -5822,7 +5833,7 @@
       <c r="AK55" s="35"/>
     </row>
     <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="89" t="n">
+      <c r="A56" s="90" t="n">
         <v>2223</v>
       </c>
       <c r="B56" s="20"/>
@@ -5887,7 +5898,7 @@
       <c r="AK56" s="35"/>
     </row>
     <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="93" t="n">
+      <c r="A57" s="94" t="n">
         <v>2311</v>
       </c>
       <c r="B57" s="44"/>
@@ -5952,7 +5963,7 @@
       <c r="AK57" s="35"/>
     </row>
     <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="93" t="n">
+      <c r="A58" s="94" t="n">
         <v>2312</v>
       </c>
       <c r="B58" s="80" t="n">
@@ -6019,13 +6030,13 @@
         <v>48</v>
       </c>
       <c r="AG58" s="55" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AH58" s="64" t="n">
         <v>30</v>
       </c>
       <c r="AI58" s="64" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="AJ58" s="82" t="s">
         <v>60</v>
@@ -6033,7 +6044,7 @@
       <c r="AK58" s="83"/>
     </row>
     <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="94" t="n">
+      <c r="A59" s="95" t="n">
         <v>2312</v>
       </c>
       <c r="B59" s="84" t="n">
@@ -6116,15 +6127,15 @@
         <v>1440</v>
       </c>
       <c r="AI59" s="64" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="AJ59" s="65" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AK59" s="83"/>
     </row>
     <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="95" t="n">
+      <c r="A60" s="96" t="n">
         <v>2312</v>
       </c>
       <c r="B60" s="86" t="n">
@@ -6191,21 +6202,21 @@
         <v>42</v>
       </c>
       <c r="AG60" s="71" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AH60" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI60" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AJ60" s="73" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AK60" s="83"/>
     </row>
     <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="95" t="n">
+      <c r="A61" s="96" t="n">
         <v>2313</v>
       </c>
       <c r="B61" s="76"/>
@@ -6270,7 +6281,7 @@
       <c r="AK61" s="35"/>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="89" t="n">
+      <c r="A62" s="90" t="n">
         <v>2321</v>
       </c>
       <c r="B62" s="20"/>
@@ -6335,7 +6346,7 @@
       <c r="AK62" s="35"/>
     </row>
     <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="89" t="n">
+      <c r="A63" s="90" t="n">
         <v>2322</v>
       </c>
       <c r="B63" s="20"/>
@@ -6400,7 +6411,7 @@
       <c r="AK63" s="35"/>
     </row>
     <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="89" t="n">
+      <c r="A64" s="90" t="n">
         <v>2323</v>
       </c>
       <c r="B64" s="20"/>
@@ -6465,7 +6476,7 @@
       <c r="AK64" s="35"/>
     </row>
     <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="89" t="n">
+      <c r="A65" s="90" t="n">
         <v>2411</v>
       </c>
       <c r="B65" s="20" t="n">
@@ -6540,13 +6551,13 @@
         <v>40</v>
       </c>
       <c r="AG65" s="25" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AH65" s="42" t="n">
         <v>30</v>
       </c>
       <c r="AI65" s="42" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="AJ65" s="27" t="s">
         <v>91</v>
@@ -6554,7 +6565,7 @@
       <c r="AK65" s="35"/>
     </row>
     <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="89" t="n">
+      <c r="A66" s="90" t="n">
         <v>2412</v>
       </c>
       <c r="B66" s="20" t="n">
@@ -6618,16 +6629,16 @@
         <v>-0.790571985844875</v>
       </c>
       <c r="AF66" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG66" s="25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AH66" s="42" t="n">
         <v>30</v>
       </c>
       <c r="AI66" s="42" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="AJ66" s="27" t="s">
         <v>86</v>
@@ -6635,7 +6646,7 @@
       <c r="AK66" s="35"/>
     </row>
     <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="89" t="n">
+      <c r="A67" s="90" t="n">
         <v>2413</v>
       </c>
       <c r="B67" s="20"/>
@@ -6700,7 +6711,7 @@
       <c r="AK67" s="35"/>
     </row>
     <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="89" t="n">
+      <c r="A68" s="90" t="n">
         <v>2421</v>
       </c>
       <c r="B68" s="20"/>
@@ -6765,7 +6776,7 @@
       <c r="AK68" s="35"/>
     </row>
     <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="89" t="n">
+      <c r="A69" s="90" t="n">
         <v>2422</v>
       </c>
       <c r="B69" s="20"/>
@@ -6830,7 +6841,7 @@
       <c r="AK69" s="35"/>
     </row>
     <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="93" t="n">
+      <c r="A70" s="94" t="n">
         <v>2423</v>
       </c>
       <c r="B70" s="44"/>
@@ -6895,7 +6906,7 @@
       <c r="AK70" s="35"/>
     </row>
     <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="96" t="n">
+      <c r="A71" s="97" t="n">
         <v>3111</v>
       </c>
       <c r="B71" s="44" t="n">
@@ -6964,61 +6975,61 @@
         <f aca="false">(Z71-AA71)/SQRT((Z71+AA71)/2*(1-(Z71+AA71)/2)*2/50)</f>
         <v>-0.0653323551323693</v>
       </c>
-      <c r="AF71" s="97" t="s">
+      <c r="AF71" s="98" t="s">
         <v>50</v>
       </c>
       <c r="AG71" s="49" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AH71" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI71" s="64" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AJ71" s="51" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AK71" s="35"/>
     </row>
     <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="88" t="n">
+      <c r="A72" s="89" t="n">
         <v>3111</v>
       </c>
-      <c r="B72" s="98" t="n">
+      <c r="B72" s="99" t="n">
         <v>0.26</v>
       </c>
-      <c r="C72" s="98" t="n">
+      <c r="C72" s="99" t="n">
         <v>0.23</v>
       </c>
-      <c r="D72" s="98"/>
-      <c r="E72" s="98"/>
-      <c r="F72" s="98"/>
-      <c r="G72" s="98"/>
-      <c r="H72" s="98"/>
-      <c r="I72" s="98"/>
-      <c r="J72" s="98"/>
-      <c r="K72" s="98"/>
-      <c r="L72" s="98"/>
-      <c r="M72" s="98"/>
-      <c r="N72" s="99" t="n">
+      <c r="D72" s="99"/>
+      <c r="E72" s="99"/>
+      <c r="F72" s="99"/>
+      <c r="G72" s="99"/>
+      <c r="H72" s="99"/>
+      <c r="I72" s="99"/>
+      <c r="J72" s="99"/>
+      <c r="K72" s="99"/>
+      <c r="L72" s="99"/>
+      <c r="M72" s="99"/>
+      <c r="N72" s="100" t="n">
         <v>0.23</v>
       </c>
-      <c r="O72" s="99" t="n">
+      <c r="O72" s="100" t="n">
         <v>0.2</v>
       </c>
-      <c r="P72" s="99" t="n">
+      <c r="P72" s="100" t="n">
         <v>0.2</v>
       </c>
-      <c r="Q72" s="99" t="n">
+      <c r="Q72" s="100" t="n">
         <v>0.29</v>
       </c>
-      <c r="R72" s="99"/>
-      <c r="S72" s="99"/>
-      <c r="T72" s="99"/>
-      <c r="U72" s="99"/>
-      <c r="V72" s="99"/>
-      <c r="W72" s="99"/>
+      <c r="R72" s="100"/>
+      <c r="S72" s="100"/>
+      <c r="T72" s="100"/>
+      <c r="U72" s="100"/>
+      <c r="V72" s="100"/>
+      <c r="W72" s="100"/>
       <c r="X72" s="60" t="n">
         <f aca="false">AVERAGE(B72:M72)</f>
         <v>0.245</v>
@@ -7051,61 +7062,61 @@
         <f aca="false">(Z72-AA72)/SQRT((Z72+AA72)/2*(1-(Z72+AA72)/2)*2/50)</f>
         <v>0.0772091436482189</v>
       </c>
-      <c r="AF72" s="100" t="s">
+      <c r="AF72" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="AG72" s="101" t="s">
-        <v>120</v>
+      <c r="AG72" s="102" t="s">
+        <v>122</v>
       </c>
       <c r="AH72" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI72" s="64" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ72" s="65" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AK72" s="35"/>
     </row>
     <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="88" t="n">
+      <c r="A73" s="89" t="n">
         <v>3111</v>
       </c>
-      <c r="B73" s="98" t="n">
+      <c r="B73" s="99" t="n">
         <v>0.4</v>
       </c>
-      <c r="C73" s="98" t="n">
+      <c r="C73" s="99" t="n">
         <v>0.58</v>
       </c>
-      <c r="D73" s="98"/>
-      <c r="E73" s="98"/>
-      <c r="F73" s="98"/>
-      <c r="G73" s="98"/>
-      <c r="H73" s="98"/>
-      <c r="I73" s="98"/>
-      <c r="J73" s="98"/>
-      <c r="K73" s="98"/>
-      <c r="L73" s="98"/>
-      <c r="M73" s="98"/>
-      <c r="N73" s="99" t="n">
+      <c r="D73" s="99"/>
+      <c r="E73" s="99"/>
+      <c r="F73" s="99"/>
+      <c r="G73" s="99"/>
+      <c r="H73" s="99"/>
+      <c r="I73" s="99"/>
+      <c r="J73" s="99"/>
+      <c r="K73" s="99"/>
+      <c r="L73" s="99"/>
+      <c r="M73" s="99"/>
+      <c r="N73" s="100" t="n">
         <v>0.39</v>
       </c>
-      <c r="O73" s="99" t="n">
+      <c r="O73" s="100" t="n">
         <v>0.37</v>
       </c>
-      <c r="P73" s="99" t="n">
+      <c r="P73" s="100" t="n">
         <v>0.48</v>
       </c>
-      <c r="Q73" s="99" t="n">
+      <c r="Q73" s="100" t="n">
         <v>0.58</v>
       </c>
-      <c r="R73" s="99"/>
-      <c r="S73" s="99"/>
-      <c r="T73" s="99"/>
-      <c r="U73" s="99"/>
-      <c r="V73" s="99"/>
-      <c r="W73" s="99"/>
+      <c r="R73" s="100"/>
+      <c r="S73" s="100"/>
+      <c r="T73" s="100"/>
+      <c r="U73" s="100"/>
+      <c r="V73" s="100"/>
+      <c r="W73" s="100"/>
       <c r="X73" s="60" t="n">
         <f aca="false">AVERAGE(B73:M73)</f>
         <v>0.49</v>
@@ -7138,25 +7149,25 @@
         <f aca="false">(Z73-AA73)/SQRT((Z73+AA73)/2*(1-(Z73+AA73)/2)*2/50)</f>
         <v>0.198563383692048</v>
       </c>
-      <c r="AF73" s="100" t="s">
+      <c r="AF73" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="AG73" s="101" t="s">
-        <v>122</v>
+      <c r="AG73" s="102" t="s">
+        <v>124</v>
       </c>
       <c r="AH73" s="50" t="n">
         <v>120</v>
       </c>
       <c r="AI73" s="50" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="AJ73" s="65" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AK73" s="35"/>
     </row>
     <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="94" t="n">
+      <c r="A74" s="95" t="n">
         <v>3111</v>
       </c>
       <c r="B74" s="84" t="n">
@@ -7228,24 +7239,24 @@
         <v>0.74635505526611</v>
       </c>
       <c r="AF74" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG74" s="63" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AH74" s="64" t="n">
         <v>30</v>
       </c>
       <c r="AI74" s="64" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="AJ74" s="65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AK74" s="83"/>
     </row>
     <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="94" t="n">
+      <c r="A75" s="95" t="n">
         <v>3111</v>
       </c>
       <c r="B75" s="84" t="n">
@@ -7317,24 +7328,24 @@
         <v>0.12778115455772</v>
       </c>
       <c r="AF75" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG75" s="71" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AH75" s="72" t="n">
         <v>180</v>
       </c>
       <c r="AI75" s="72" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AJ75" s="73" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AK75" s="83"/>
     </row>
     <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="96" t="n">
+      <c r="A76" s="97" t="n">
         <v>3112</v>
       </c>
       <c r="B76" s="80" t="n">
@@ -7401,21 +7412,21 @@
         <v>50</v>
       </c>
       <c r="AG76" s="55" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AH76" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI76" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ76" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="AJ76" s="82" t="s">
-        <v>108</v>
-      </c>
       <c r="AK76" s="83"/>
     </row>
     <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="88" t="n">
+      <c r="A77" s="89" t="n">
         <v>3112</v>
       </c>
       <c r="B77" s="84" t="n">
@@ -7482,21 +7493,21 @@
         <v>50</v>
       </c>
       <c r="AG77" s="63" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AH77" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI77" s="64" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AJ77" s="65" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK77" s="83"/>
     </row>
     <row r="78" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="88" t="n">
+      <c r="A78" s="89" t="n">
         <v>3112</v>
       </c>
       <c r="B78" s="84" t="n">
@@ -7563,21 +7574,21 @@
         <v>50</v>
       </c>
       <c r="AG78" s="63" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AH78" s="64" t="n">
         <v>30</v>
       </c>
       <c r="AI78" s="64" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="AJ78" s="65" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK78" s="83"/>
     </row>
     <row r="79" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="88" t="n">
+      <c r="A79" s="89" t="n">
         <v>3112</v>
       </c>
       <c r="B79" s="84" t="n">
@@ -7649,24 +7660,24 @@
         <v>-1.11012311498065</v>
       </c>
       <c r="AF79" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG79" s="63" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AH79" s="64" t="n">
         <v>30</v>
       </c>
       <c r="AI79" s="64" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="AJ79" s="65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AK79" s="83"/>
     </row>
     <row r="80" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="88" t="n">
+      <c r="A80" s="89" t="n">
         <v>3112</v>
       </c>
       <c r="B80" s="84" t="n">
@@ -7732,24 +7743,24 @@
         <v>-1.15512696152572</v>
       </c>
       <c r="AF80" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG80" s="63" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AH80" s="64" t="n">
         <v>180</v>
       </c>
       <c r="AI80" s="64" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="AJ80" s="65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AK80" s="83"/>
     </row>
     <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="88" t="n">
+      <c r="A81" s="89" t="n">
         <v>3112</v>
       </c>
       <c r="B81" s="84" t="n">
@@ -7821,24 +7832,24 @@
         <v>-1.45282175323828</v>
       </c>
       <c r="AF81" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG81" s="63" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AH81" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI81" s="64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AJ81" s="65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AK81" s="83"/>
     </row>
     <row r="82" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="88" t="n">
+      <c r="A82" s="89" t="n">
         <v>3112</v>
       </c>
       <c r="B82" s="84" t="n">
@@ -7902,24 +7913,24 @@
         <v>0.0775116171167646</v>
       </c>
       <c r="AF82" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG82" s="63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH82" s="64" t="n">
         <v>180</v>
       </c>
       <c r="AI82" s="64" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ82" s="65" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AK82" s="83"/>
     </row>
     <row r="83" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="102" t="n">
+      <c r="A83" s="103" t="n">
         <v>3112</v>
       </c>
       <c r="B83" s="86" t="n">
@@ -7983,7 +7994,7 @@
         <v>-0.907702771299795</v>
       </c>
       <c r="AF83" s="70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG83" s="71" t="s">
         <v>92</v>
@@ -7992,39 +8003,39 @@
         <v>180</v>
       </c>
       <c r="AI83" s="72" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="AJ83" s="73" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AK83" s="83"/>
     </row>
     <row r="84" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="88" t="n">
+      <c r="A84" s="89" t="n">
         <v>3113</v>
       </c>
-      <c r="B84" s="98"/>
-      <c r="C84" s="98"/>
-      <c r="D84" s="98"/>
-      <c r="E84" s="98"/>
-      <c r="F84" s="98"/>
-      <c r="G84" s="98"/>
-      <c r="H84" s="98"/>
-      <c r="I84" s="98"/>
-      <c r="J84" s="98"/>
-      <c r="K84" s="98"/>
-      <c r="L84" s="98"/>
-      <c r="M84" s="98"/>
-      <c r="N84" s="99"/>
-      <c r="O84" s="99"/>
-      <c r="P84" s="99"/>
-      <c r="Q84" s="99"/>
-      <c r="R84" s="99"/>
-      <c r="S84" s="99"/>
-      <c r="T84" s="99"/>
-      <c r="U84" s="99"/>
-      <c r="V84" s="99"/>
-      <c r="W84" s="99"/>
+      <c r="B84" s="99"/>
+      <c r="C84" s="99"/>
+      <c r="D84" s="99"/>
+      <c r="E84" s="99"/>
+      <c r="F84" s="99"/>
+      <c r="G84" s="99"/>
+      <c r="H84" s="99"/>
+      <c r="I84" s="99"/>
+      <c r="J84" s="99"/>
+      <c r="K84" s="99"/>
+      <c r="L84" s="99"/>
+      <c r="M84" s="99"/>
+      <c r="N84" s="100"/>
+      <c r="O84" s="100"/>
+      <c r="P84" s="100"/>
+      <c r="Q84" s="100"/>
+      <c r="R84" s="100"/>
+      <c r="S84" s="100"/>
+      <c r="T84" s="100"/>
+      <c r="U84" s="100"/>
+      <c r="V84" s="100"/>
+      <c r="W84" s="100"/>
       <c r="X84" s="60" t="e">
         <f aca="false">AVERAGE(B84:M84)</f>
         <v>#DIV/0!</v>
@@ -8065,7 +8076,7 @@
       <c r="AK84" s="35"/>
     </row>
     <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="96" t="n">
+      <c r="A85" s="97" t="n">
         <v>3121</v>
       </c>
       <c r="B85" s="44" t="n">
@@ -8128,63 +8139,63 @@
         <f aca="false">(Z85-AA85)/SQRT((Z85+AA85)/2*(1-(Z85+AA85)/2)*2/50)</f>
         <v>-0.0774083364133037</v>
       </c>
-      <c r="AF85" s="97" t="s">
-        <v>135</v>
+      <c r="AF85" s="98" t="s">
+        <v>137</v>
       </c>
       <c r="AG85" s="49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AH85" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI85" s="64" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="AJ85" s="51" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK85" s="35"/>
     </row>
     <row r="86" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="94" t="n">
+      <c r="A86" s="95" t="n">
         <v>3121</v>
       </c>
-      <c r="B86" s="98" t="n">
+      <c r="B86" s="99" t="n">
         <v>-0.1</v>
       </c>
-      <c r="C86" s="98" t="n">
+      <c r="C86" s="99" t="n">
         <v>-0.24</v>
       </c>
-      <c r="D86" s="98"/>
-      <c r="E86" s="98"/>
-      <c r="F86" s="98"/>
-      <c r="G86" s="98"/>
-      <c r="H86" s="98"/>
-      <c r="I86" s="98"/>
-      <c r="J86" s="98"/>
-      <c r="K86" s="98"/>
-      <c r="L86" s="98"/>
-      <c r="M86" s="98"/>
-      <c r="N86" s="99" t="n">
+      <c r="D86" s="99"/>
+      <c r="E86" s="99"/>
+      <c r="F86" s="99"/>
+      <c r="G86" s="99"/>
+      <c r="H86" s="99"/>
+      <c r="I86" s="99"/>
+      <c r="J86" s="99"/>
+      <c r="K86" s="99"/>
+      <c r="L86" s="99"/>
+      <c r="M86" s="99"/>
+      <c r="N86" s="100" t="n">
         <v>-0.41</v>
       </c>
-      <c r="O86" s="99" t="n">
+      <c r="O86" s="100" t="n">
         <v>-0.39</v>
       </c>
-      <c r="P86" s="99" t="n">
+      <c r="P86" s="100" t="n">
         <v>-0.34</v>
       </c>
-      <c r="Q86" s="99" t="n">
+      <c r="Q86" s="100" t="n">
         <v>-0.45</v>
       </c>
-      <c r="R86" s="99" t="n">
+      <c r="R86" s="100" t="n">
         <v>-0.42</v>
       </c>
-      <c r="S86" s="99"/>
-      <c r="T86" s="99"/>
-      <c r="U86" s="99"/>
-      <c r="V86" s="99"/>
-      <c r="W86" s="99"/>
+      <c r="S86" s="100"/>
+      <c r="T86" s="100"/>
+      <c r="U86" s="100"/>
+      <c r="V86" s="100"/>
+      <c r="W86" s="100"/>
       <c r="X86" s="60" t="n">
         <f aca="false">AVERAGE(B86:M86)</f>
         <v>-0.17</v>
@@ -8218,24 +8229,24 @@
         <v>1.21056579625906</v>
       </c>
       <c r="AF86" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG86" s="71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AH86" s="42" t="n">
         <v>30</v>
       </c>
       <c r="AI86" s="42" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="AJ86" s="73" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AK86" s="35"/>
     </row>
     <row r="87" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="93" t="n">
+      <c r="A87" s="94" t="n">
         <v>3122</v>
       </c>
       <c r="B87" s="80" t="n">
@@ -8302,21 +8313,21 @@
         <v>50</v>
       </c>
       <c r="AG87" s="55" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AH87" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI87" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AJ87" s="82" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK87" s="83"/>
     </row>
     <row r="88" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="94" t="n">
+      <c r="A88" s="95" t="n">
         <v>3122</v>
       </c>
       <c r="B88" s="84" t="n">
@@ -8383,21 +8394,21 @@
         <v>50</v>
       </c>
       <c r="AG88" s="63" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AH88" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI88" s="64" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="AJ88" s="65" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AK88" s="83"/>
     </row>
     <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="94" t="n">
+      <c r="A89" s="95" t="n">
         <v>3122</v>
       </c>
       <c r="B89" s="84" t="n">
@@ -8469,24 +8480,24 @@
         <v>0.728121687423505</v>
       </c>
       <c r="AF89" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG89" s="63" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AH89" s="64" t="n">
         <v>180</v>
       </c>
       <c r="AI89" s="64" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="AJ89" s="65" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AK89" s="83"/>
     </row>
     <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="95" t="n">
+      <c r="A90" s="96" t="n">
         <v>3122</v>
       </c>
       <c r="B90" s="86" t="n">
@@ -8558,24 +8569,24 @@
         <v>0.509048943689028</v>
       </c>
       <c r="AF90" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG90" s="71" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AH90" s="72" t="n">
         <v>180</v>
       </c>
       <c r="AI90" s="72" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="AJ90" s="73" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AK90" s="83"/>
     </row>
     <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="95" t="n">
+      <c r="A91" s="96" t="n">
         <v>3123</v>
       </c>
       <c r="B91" s="76"/>
@@ -8640,7 +8651,7 @@
       <c r="AK91" s="35"/>
     </row>
     <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="93" t="n">
+      <c r="A92" s="94" t="n">
         <v>3211</v>
       </c>
       <c r="B92" s="44" t="n">
@@ -8704,24 +8715,24 @@
         <v>0.726912935085673</v>
       </c>
       <c r="AF92" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG92" s="25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AH92" s="42" t="n">
         <v>120</v>
       </c>
       <c r="AI92" s="42" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AJ92" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AK92" s="35"/>
     </row>
     <row r="93" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="93" t="n">
+      <c r="A93" s="94" t="n">
         <v>3212</v>
       </c>
       <c r="B93" s="80" t="n">
@@ -8792,13 +8803,13 @@
         <v>42</v>
       </c>
       <c r="AG93" s="55" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AH93" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI93" s="64" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="AJ93" s="82" t="s">
         <v>45</v>
@@ -8806,7 +8817,7 @@
       <c r="AK93" s="83"/>
     </row>
     <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="94" t="n">
+      <c r="A94" s="95" t="n">
         <v>3212</v>
       </c>
       <c r="B94" s="84" t="n">
@@ -8870,24 +8881,24 @@
         <v>-1.07824297529924</v>
       </c>
       <c r="AF94" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG94" s="63" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AH94" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI94" s="64" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AJ94" s="65" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AK94" s="83"/>
     </row>
     <row r="95" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="94" t="n">
+      <c r="A95" s="95" t="n">
         <v>3212</v>
       </c>
       <c r="B95" s="84" t="n">
@@ -8951,24 +8962,24 @@
         <v>-0.961621708018124</v>
       </c>
       <c r="AF95" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG95" s="63" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AH95" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI95" s="64" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AJ95" s="65" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AK95" s="83"/>
     </row>
     <row r="96" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="94" t="n">
+      <c r="A96" s="95" t="n">
         <v>3212</v>
       </c>
       <c r="B96" s="84" t="n">
@@ -9032,24 +9043,24 @@
         <v>-0.964277632972672</v>
       </c>
       <c r="AF96" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG96" s="63" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AH96" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI96" s="64" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="AJ96" s="65" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AK96" s="83"/>
     </row>
     <row r="97" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="95" t="n">
+      <c r="A97" s="96" t="n">
         <v>3212</v>
       </c>
       <c r="B97" s="86" t="n">
@@ -9113,24 +9124,24 @@
         <v>-0.702250809666986</v>
       </c>
       <c r="AF97" s="70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG97" s="71" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AH97" s="72" t="n">
         <v>120</v>
       </c>
       <c r="AI97" s="72" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="AJ97" s="73" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AK97" s="83"/>
     </row>
     <row r="98" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="95" t="n">
+      <c r="A98" s="96" t="n">
         <v>3213</v>
       </c>
       <c r="B98" s="76"/>
@@ -9195,7 +9206,7 @@
       <c r="AK98" s="35"/>
     </row>
     <row r="99" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="89" t="n">
+      <c r="A99" s="90" t="n">
         <v>3221</v>
       </c>
       <c r="B99" s="20"/>
@@ -9260,7 +9271,7 @@
       <c r="AK99" s="35"/>
     </row>
     <row r="100" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="89" t="n">
+      <c r="A100" s="90" t="n">
         <v>3222</v>
       </c>
       <c r="B100" s="20"/>
@@ -9325,31 +9336,31 @@
       <c r="AK100" s="35"/>
     </row>
     <row r="101" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="89" t="n">
+      <c r="A101" s="90" t="n">
         <v>3223</v>
       </c>
-      <c r="B101" s="103"/>
-      <c r="C101" s="103"/>
-      <c r="D101" s="103"/>
-      <c r="E101" s="103"/>
-      <c r="F101" s="103"/>
-      <c r="G101" s="103"/>
-      <c r="H101" s="103"/>
-      <c r="I101" s="103"/>
-      <c r="J101" s="103"/>
-      <c r="K101" s="103"/>
-      <c r="L101" s="103"/>
-      <c r="M101" s="103"/>
-      <c r="N101" s="104"/>
-      <c r="O101" s="104"/>
-      <c r="P101" s="104"/>
-      <c r="Q101" s="104"/>
-      <c r="R101" s="104"/>
-      <c r="S101" s="104"/>
-      <c r="T101" s="104"/>
-      <c r="U101" s="104"/>
-      <c r="V101" s="104"/>
-      <c r="W101" s="104"/>
+      <c r="B101" s="104"/>
+      <c r="C101" s="104"/>
+      <c r="D101" s="104"/>
+      <c r="E101" s="104"/>
+      <c r="F101" s="104"/>
+      <c r="G101" s="104"/>
+      <c r="H101" s="104"/>
+      <c r="I101" s="104"/>
+      <c r="J101" s="104"/>
+      <c r="K101" s="104"/>
+      <c r="L101" s="104"/>
+      <c r="M101" s="104"/>
+      <c r="N101" s="105"/>
+      <c r="O101" s="105"/>
+      <c r="P101" s="105"/>
+      <c r="Q101" s="105"/>
+      <c r="R101" s="105"/>
+      <c r="S101" s="105"/>
+      <c r="T101" s="105"/>
+      <c r="U101" s="105"/>
+      <c r="V101" s="105"/>
+      <c r="W101" s="105"/>
       <c r="X101" s="22" t="e">
         <f aca="false">AVERAGE(B101:M101)</f>
         <v>#DIV/0!</v>
@@ -9382,15 +9393,15 @@
         <f aca="false">(Z101-AA101)/SQRT((Z101+AA101)/2*(1-(Z101+AA101)/2)*2/50)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF101" s="105"/>
-      <c r="AG101" s="106"/>
+      <c r="AF101" s="106"/>
+      <c r="AG101" s="107"/>
       <c r="AH101" s="72"/>
       <c r="AI101" s="72"/>
       <c r="AJ101" s="27"/>
       <c r="AK101" s="35"/>
     </row>
     <row r="102" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="93" t="n">
+      <c r="A102" s="94" t="n">
         <v>3311</v>
       </c>
       <c r="B102" s="44"/>
@@ -9455,7 +9466,7 @@
       <c r="AK102" s="35"/>
     </row>
     <row r="103" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="93" t="n">
+      <c r="A103" s="94" t="n">
         <v>3312</v>
       </c>
       <c r="B103" s="80" t="n">
@@ -9522,13 +9533,13 @@
         <v>48</v>
       </c>
       <c r="AG103" s="55" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AH103" s="64" t="n">
         <v>30</v>
       </c>
       <c r="AI103" s="64" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="AJ103" s="82" t="s">
         <v>60</v>
@@ -9536,7 +9547,7 @@
       <c r="AK103" s="83"/>
     </row>
     <row r="104" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="94" t="n">
+      <c r="A104" s="95" t="n">
         <v>3312</v>
       </c>
       <c r="B104" s="84" t="n">
@@ -9615,13 +9626,13 @@
         <v>54</v>
       </c>
       <c r="AG104" s="63" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AH104" s="64" t="n">
         <v>30</v>
       </c>
       <c r="AI104" s="64" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="AJ104" s="65" t="s">
         <v>60</v>
@@ -9629,7 +9640,7 @@
       <c r="AK104" s="83"/>
     </row>
     <row r="105" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="102" t="n">
+      <c r="A105" s="103" t="n">
         <v>3312</v>
       </c>
       <c r="B105" s="86" t="n">
@@ -9696,21 +9707,21 @@
         <v>42</v>
       </c>
       <c r="AG105" s="71" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AH105" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI105" s="64" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="AJ105" s="73" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AK105" s="83"/>
     </row>
     <row r="106" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="95" t="n">
+      <c r="A106" s="96" t="n">
         <v>3313</v>
       </c>
       <c r="B106" s="76"/>
@@ -9775,7 +9786,7 @@
       <c r="AK106" s="35"/>
     </row>
     <row r="107" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="89" t="n">
+      <c r="A107" s="90" t="n">
         <v>3321</v>
       </c>
       <c r="B107" s="20"/>
@@ -9840,7 +9851,7 @@
       <c r="AK107" s="35"/>
     </row>
     <row r="108" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="89" t="n">
+      <c r="A108" s="90" t="n">
         <v>3322</v>
       </c>
       <c r="B108" s="20"/>
@@ -9905,7 +9916,7 @@
       <c r="AK108" s="35"/>
     </row>
     <row r="109" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="89" t="n">
+      <c r="A109" s="90" t="n">
         <v>3323</v>
       </c>
       <c r="B109" s="20"/>
@@ -9970,7 +9981,7 @@
       <c r="AK109" s="35"/>
     </row>
     <row r="110" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="93" t="n">
+      <c r="A110" s="94" t="n">
         <v>3411</v>
       </c>
       <c r="B110" s="44"/>
@@ -10035,7 +10046,7 @@
       <c r="AK110" s="35"/>
     </row>
     <row r="111" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="93" t="n">
+      <c r="A111" s="94" t="n">
         <v>3412</v>
       </c>
       <c r="B111" s="80" t="n">
@@ -10101,10 +10112,10 @@
         <v>0.705991044344285</v>
       </c>
       <c r="AF111" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG111" s="55" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AH111" s="64" t="n">
         <v>180</v>
@@ -10113,12 +10124,12 @@
         <v>93</v>
       </c>
       <c r="AJ111" s="82" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AK111" s="83"/>
     </row>
     <row r="112" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="88" t="n">
+      <c r="A112" s="89" t="n">
         <v>3412</v>
       </c>
       <c r="B112" s="84" t="n">
@@ -10184,10 +10195,10 @@
         <v>0.194333247934686</v>
       </c>
       <c r="AF112" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG112" s="63" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AH112" s="64" t="n">
         <v>180</v>
@@ -10196,12 +10207,12 @@
         <v>93</v>
       </c>
       <c r="AJ112" s="65" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AK112" s="83"/>
     </row>
     <row r="113" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="95" t="n">
+      <c r="A113" s="96" t="n">
         <v>3412</v>
       </c>
       <c r="B113" s="86" t="n">
@@ -10265,24 +10276,24 @@
         <v>0.101477094257997</v>
       </c>
       <c r="AF113" s="70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG113" s="71" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AH113" s="72" t="n">
         <v>180</v>
       </c>
       <c r="AI113" s="72" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="AJ113" s="73" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AK113" s="83"/>
     </row>
     <row r="114" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="95" t="n">
+      <c r="A114" s="96" t="n">
         <v>3413</v>
       </c>
       <c r="B114" s="76"/>
@@ -10347,7 +10358,7 @@
       <c r="AK114" s="35"/>
     </row>
     <row r="115" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="89" t="n">
+      <c r="A115" s="90" t="n">
         <v>3421</v>
       </c>
       <c r="B115" s="20"/>
@@ -10412,7 +10423,7 @@
       <c r="AK115" s="35"/>
     </row>
     <row r="116" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="89" t="n">
+      <c r="A116" s="90" t="n">
         <v>3422</v>
       </c>
       <c r="B116" s="20"/>
@@ -10477,7 +10488,7 @@
       <c r="AK116" s="35"/>
     </row>
     <row r="117" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="93" t="n">
+      <c r="A117" s="94" t="n">
         <v>3423</v>
       </c>
       <c r="B117" s="44"/>
@@ -10542,7 +10553,7 @@
       <c r="AK117" s="35"/>
     </row>
     <row r="118" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="107" t="n">
+      <c r="A118" s="108" t="n">
         <f aca="false">A74+1000</f>
         <v>4111</v>
       </c>
@@ -10620,13 +10631,13 @@
         <v>52</v>
       </c>
       <c r="AG118" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AH118" s="56" t="n">
         <v>120</v>
       </c>
       <c r="AI118" s="56" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="AJ118" s="82" t="s">
         <v>163</v>
@@ -10634,7 +10645,7 @@
       <c r="AK118" s="83"/>
     </row>
     <row r="119" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="108" t="n">
+      <c r="A119" s="109" t="n">
         <v>4111</v>
       </c>
       <c r="B119" s="84" t="n">
@@ -10717,7 +10728,7 @@
         <v>1.5</v>
       </c>
       <c r="AI119" s="64" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AJ119" s="65" t="s">
         <v>165</v>
@@ -10725,7 +10736,7 @@
       <c r="AK119" s="83"/>
     </row>
     <row r="120" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="108" t="n">
+      <c r="A120" s="109" t="n">
         <v>4111</v>
       </c>
       <c r="B120" s="84" t="n">
@@ -10802,13 +10813,13 @@
         <v>52</v>
       </c>
       <c r="AG120" s="63" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AH120" s="64" t="n">
         <v>1.5</v>
       </c>
       <c r="AI120" s="64" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ120" s="65" t="s">
         <v>166</v>
@@ -10816,7 +10827,7 @@
       <c r="AK120" s="83"/>
     </row>
     <row r="121" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="109" t="n">
+      <c r="A121" s="110" t="n">
         <f aca="false">A75+1000</f>
         <v>4111</v>
       </c>
@@ -10886,13 +10897,13 @@
         <v>52</v>
       </c>
       <c r="AG121" s="63" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AH121" s="72" t="n">
         <v>120</v>
       </c>
       <c r="AI121" s="72" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ121" s="65" t="s">
         <v>167</v>
@@ -10900,7 +10911,7 @@
       <c r="AK121" s="83"/>
     </row>
     <row r="122" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="110" t="n">
+      <c r="A122" s="111" t="n">
         <v>4112</v>
       </c>
       <c r="B122" s="80" t="n">
@@ -10967,21 +10978,21 @@
         <v>50</v>
       </c>
       <c r="AG122" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH122" s="64" t="n">
         <v>1440</v>
       </c>
       <c r="AI122" s="64" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="AJ122" s="82" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AK122" s="83"/>
     </row>
     <row r="123" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="109" t="n">
+      <c r="A123" s="110" t="n">
         <f aca="false">A76+1000</f>
         <v>4112</v>
       </c>
@@ -11055,21 +11066,21 @@
         <v>50</v>
       </c>
       <c r="AG123" s="63" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AH123" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI123" s="64" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ123" s="65" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AK123" s="83"/>
     </row>
     <row r="124" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="109" t="n">
+      <c r="A124" s="110" t="n">
         <f aca="false">A78+1000</f>
         <v>4112</v>
       </c>
@@ -11147,21 +11158,21 @@
         <v>52</v>
       </c>
       <c r="AG124" s="63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AH124" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI124" s="64" t="s">
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="AJ124" s="65" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AK124" s="83"/>
     </row>
     <row r="125" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="111" t="n">
+      <c r="A125" s="112" t="n">
         <f aca="false">A79+1000</f>
         <v>4112</v>
       </c>
@@ -11247,21 +11258,21 @@
         <v>52</v>
       </c>
       <c r="AG125" s="71" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AH125" s="72" t="n">
         <v>120</v>
       </c>
       <c r="AI125" s="72" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ125" s="73" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AK125" s="83"/>
     </row>
     <row r="126" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="111" t="n">
+      <c r="A126" s="112" t="n">
         <f aca="false">A84+1000</f>
         <v>4113</v>
       </c>
@@ -11325,14 +11336,14 @@
       <c r="AI126" s="42"/>
       <c r="AJ126" s="27"/>
       <c r="AK126" s="35"/>
-      <c r="AL126" s="112"/>
-      <c r="AM126" s="112"/>
-      <c r="AN126" s="112"/>
-      <c r="AO126" s="112"/>
-      <c r="AP126" s="112"/>
+      <c r="AL126" s="113"/>
+      <c r="AM126" s="113"/>
+      <c r="AN126" s="113"/>
+      <c r="AO126" s="113"/>
+      <c r="AP126" s="113"/>
     </row>
     <row r="127" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="113" t="n">
+      <c r="A127" s="114" t="n">
         <f aca="false">A86+1000</f>
         <v>4121</v>
       </c>
@@ -11396,14 +11407,14 @@
       <c r="AI127" s="42"/>
       <c r="AJ127" s="27"/>
       <c r="AK127" s="35"/>
-      <c r="AL127" s="112"/>
-      <c r="AM127" s="112"/>
-      <c r="AN127" s="112"/>
-      <c r="AO127" s="112"/>
-      <c r="AP127" s="112"/>
+      <c r="AL127" s="113"/>
+      <c r="AM127" s="113"/>
+      <c r="AN127" s="113"/>
+      <c r="AO127" s="113"/>
+      <c r="AP127" s="113"/>
     </row>
     <row r="128" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="113" t="n">
+      <c r="A128" s="114" t="n">
         <f aca="false">A87+1000</f>
         <v>4122</v>
       </c>
@@ -11467,14 +11478,14 @@
       <c r="AI128" s="42"/>
       <c r="AJ128" s="27"/>
       <c r="AK128" s="35"/>
-      <c r="AL128" s="112"/>
-      <c r="AM128" s="112"/>
-      <c r="AN128" s="112"/>
-      <c r="AO128" s="112"/>
-      <c r="AP128" s="112"/>
+      <c r="AL128" s="113"/>
+      <c r="AM128" s="113"/>
+      <c r="AN128" s="113"/>
+      <c r="AO128" s="113"/>
+      <c r="AP128" s="113"/>
     </row>
     <row r="129" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="107" t="n">
+      <c r="A129" s="108" t="n">
         <f aca="false">A91+1000</f>
         <v>4123</v>
       </c>
@@ -11538,14 +11549,14 @@
       <c r="AI129" s="50"/>
       <c r="AJ129" s="51"/>
       <c r="AK129" s="35"/>
-      <c r="AL129" s="112"/>
-      <c r="AM129" s="112"/>
-      <c r="AN129" s="112"/>
-      <c r="AO129" s="112"/>
-      <c r="AP129" s="112"/>
+      <c r="AL129" s="113"/>
+      <c r="AM129" s="113"/>
+      <c r="AN129" s="113"/>
+      <c r="AO129" s="113"/>
+      <c r="AP129" s="113"/>
     </row>
     <row r="130" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="110" t="n">
+      <c r="A130" s="111" t="n">
         <v>4211</v>
       </c>
       <c r="B130" s="80" t="n">
@@ -11612,34 +11623,34 @@
         <f aca="false">COUNTIF(N130:W130,"&gt;0")+COUNTIF(N130:W130,"&lt;=0")</f>
         <v>1</v>
       </c>
-      <c r="AE130" s="114" t="n">
+      <c r="AE130" s="115" t="n">
         <f aca="false">(Z130-AA130)/SQRT((Z130+AA130)/2*(1-(Z130+AA130)/2)*2/50)</f>
         <v>0.276456093031517</v>
       </c>
-      <c r="AF130" s="115" t="s">
+      <c r="AF130" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="AG130" s="116" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH130" s="117" t="n">
+      <c r="AG130" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH130" s="118" t="n">
         <v>1.5</v>
       </c>
-      <c r="AI130" s="117" t="s">
-        <v>107</v>
+      <c r="AI130" s="118" t="s">
+        <v>109</v>
       </c>
       <c r="AJ130" s="51" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AK130" s="35"/>
-      <c r="AL130" s="112"/>
-      <c r="AM130" s="112"/>
-      <c r="AN130" s="112"/>
-      <c r="AO130" s="112"/>
-      <c r="AP130" s="112"/>
+      <c r="AL130" s="113"/>
+      <c r="AM130" s="113"/>
+      <c r="AN130" s="113"/>
+      <c r="AO130" s="113"/>
+      <c r="AP130" s="113"/>
     </row>
     <row r="131" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="109" t="n">
+      <c r="A131" s="110" t="n">
         <f aca="false">A92+1000</f>
         <v>4211</v>
       </c>
@@ -11701,34 +11712,34 @@
         <f aca="false">COUNTIF(N131:W131,"&gt;0")+COUNTIF(N131:W131,"&lt;=0")</f>
         <v>1</v>
       </c>
-      <c r="AE131" s="118" t="n">
+      <c r="AE131" s="119" t="n">
         <f aca="false">(Z131-AA131)/SQRT((Z131+AA131)/2*(1-(Z131+AA131)/2)*2/50)</f>
         <v>0.494602561047701</v>
       </c>
-      <c r="AF131" s="119" t="s">
+      <c r="AF131" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="AG131" s="120" t="s">
-        <v>129</v>
+      <c r="AG131" s="121" t="s">
+        <v>131</v>
       </c>
       <c r="AH131" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI131" s="64" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AJ131" s="65" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AK131" s="83"/>
-      <c r="AL131" s="112"/>
-      <c r="AM131" s="112"/>
-      <c r="AN131" s="112"/>
-      <c r="AO131" s="112"/>
-      <c r="AP131" s="112"/>
+      <c r="AL131" s="113"/>
+      <c r="AM131" s="113"/>
+      <c r="AN131" s="113"/>
+      <c r="AO131" s="113"/>
+      <c r="AP131" s="113"/>
     </row>
     <row r="132" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="108" t="n">
+      <c r="A132" s="109" t="n">
         <v>4211</v>
       </c>
       <c r="B132" s="84" t="n">
@@ -11787,34 +11798,34 @@
         <f aca="false">COUNTIF(N132:W132,"&gt;0")+COUNTIF(N132:W132,"&lt;=0")</f>
         <v>2</v>
       </c>
-      <c r="AE132" s="118" t="n">
+      <c r="AE132" s="119" t="n">
         <f aca="false">(Z132-AA132)/SQRT((Z132+AA132)/2*(1-(Z132+AA132)/2)*2/50)</f>
         <v>1.69939625511031</v>
       </c>
-      <c r="AF132" s="119" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG132" s="120" t="s">
-        <v>177</v>
+      <c r="AF132" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG132" s="121" t="s">
+        <v>178</v>
       </c>
       <c r="AH132" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI132" s="64" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="AJ132" s="65" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AK132" s="83"/>
-      <c r="AL132" s="112"/>
-      <c r="AM132" s="112"/>
-      <c r="AN132" s="112"/>
-      <c r="AO132" s="112"/>
-      <c r="AP132" s="112"/>
+      <c r="AL132" s="113"/>
+      <c r="AM132" s="113"/>
+      <c r="AN132" s="113"/>
+      <c r="AO132" s="113"/>
+      <c r="AP132" s="113"/>
     </row>
     <row r="133" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="108" t="n">
+      <c r="A133" s="109" t="n">
         <v>4211</v>
       </c>
       <c r="B133" s="84" t="n">
@@ -11873,34 +11884,34 @@
         <f aca="false">COUNTIF(N133:W133,"&gt;0")+COUNTIF(N133:W133,"&lt;=0")</f>
         <v>2</v>
       </c>
-      <c r="AE133" s="118" t="n">
+      <c r="AE133" s="119" t="n">
         <f aca="false">(Z133-AA133)/SQRT((Z133+AA133)/2*(1-(Z133+AA133)/2)*2/50)</f>
         <v>1.82279724261905</v>
       </c>
-      <c r="AF133" s="119" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG133" s="120" t="s">
-        <v>178</v>
+      <c r="AF133" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG133" s="121" t="s">
+        <v>179</v>
       </c>
       <c r="AH133" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI133" s="64" t="s">
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="AJ133" s="65" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AK133" s="83"/>
-      <c r="AL133" s="112"/>
-      <c r="AM133" s="112"/>
-      <c r="AN133" s="112"/>
-      <c r="AO133" s="112"/>
-      <c r="AP133" s="112"/>
+      <c r="AL133" s="113"/>
+      <c r="AM133" s="113"/>
+      <c r="AN133" s="113"/>
+      <c r="AO133" s="113"/>
+      <c r="AP133" s="113"/>
     </row>
     <row r="134" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="108" t="n">
+      <c r="A134" s="109" t="n">
         <v>4211</v>
       </c>
       <c r="B134" s="84" t="n">
@@ -11959,34 +11970,34 @@
         <f aca="false">COUNTIF(N134:W134,"&gt;0")+COUNTIF(N134:W134,"&lt;=0")</f>
         <v>2</v>
       </c>
-      <c r="AE134" s="118" t="n">
+      <c r="AE134" s="119" t="n">
         <f aca="false">(Z134-AA134)/SQRT((Z134+AA134)/2*(1-(Z134+AA134)/2)*2/50)</f>
         <v>1.19287044528514</v>
       </c>
-      <c r="AF134" s="121" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG134" s="122" t="s">
-        <v>179</v>
+      <c r="AF134" s="122" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG134" s="123" t="s">
+        <v>180</v>
       </c>
       <c r="AH134" s="72" t="n">
         <v>3</v>
       </c>
       <c r="AI134" s="72" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AJ134" s="73" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AK134" s="83"/>
-      <c r="AL134" s="112"/>
-      <c r="AM134" s="112"/>
-      <c r="AN134" s="112"/>
-      <c r="AO134" s="112"/>
-      <c r="AP134" s="112"/>
+      <c r="AL134" s="113"/>
+      <c r="AM134" s="113"/>
+      <c r="AN134" s="113"/>
+      <c r="AO134" s="113"/>
+      <c r="AP134" s="113"/>
     </row>
     <row r="135" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="107" t="n">
+      <c r="A135" s="108" t="n">
         <f aca="false">A93+1000</f>
         <v>4212</v>
       </c>
@@ -12058,26 +12069,26 @@
         <v>52</v>
       </c>
       <c r="AG135" s="55" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AH135" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI135" s="64" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="AJ135" s="82" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AK135" s="83"/>
-      <c r="AL135" s="112"/>
-      <c r="AM135" s="112"/>
-      <c r="AN135" s="112"/>
-      <c r="AO135" s="112"/>
-      <c r="AP135" s="112"/>
+      <c r="AL135" s="113"/>
+      <c r="AM135" s="113"/>
+      <c r="AN135" s="113"/>
+      <c r="AO135" s="113"/>
+      <c r="AP135" s="113"/>
     </row>
     <row r="136" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="109" t="n">
+      <c r="A136" s="110" t="n">
         <f aca="false">A94+1000</f>
         <v>4212</v>
       </c>
@@ -12157,26 +12168,26 @@
         <v>52</v>
       </c>
       <c r="AG136" s="63" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AH136" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI136" s="64" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ136" s="65" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AK136" s="83"/>
-      <c r="AL136" s="112"/>
-      <c r="AM136" s="112"/>
-      <c r="AN136" s="112"/>
-      <c r="AO136" s="112"/>
-      <c r="AP136" s="112"/>
+      <c r="AL136" s="113"/>
+      <c r="AM136" s="113"/>
+      <c r="AN136" s="113"/>
+      <c r="AO136" s="113"/>
+      <c r="AP136" s="113"/>
     </row>
     <row r="137" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="109" t="n">
+      <c r="A137" s="110" t="n">
         <f aca="false">A95+1000</f>
         <v>4212</v>
       </c>
@@ -12248,26 +12259,26 @@
         <v>42</v>
       </c>
       <c r="AG137" s="63" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH137" s="64" t="n">
         <v>5</v>
       </c>
       <c r="AI137" s="64" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AJ137" s="65" t="s">
         <v>45</v>
       </c>
       <c r="AK137" s="83"/>
-      <c r="AL137" s="112"/>
-      <c r="AM137" s="112"/>
-      <c r="AN137" s="112"/>
-      <c r="AO137" s="112"/>
-      <c r="AP137" s="112"/>
+      <c r="AL137" s="113"/>
+      <c r="AM137" s="113"/>
+      <c r="AN137" s="113"/>
+      <c r="AO137" s="113"/>
+      <c r="AP137" s="113"/>
     </row>
     <row r="138" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="109" t="n">
+      <c r="A138" s="110" t="n">
         <f aca="false">A97+1000</f>
         <v>4212</v>
       </c>
@@ -12332,29 +12343,29 @@
         <v>-1.14939328522415</v>
       </c>
       <c r="AF138" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG138" s="63" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH138" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI138" s="64" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="AJ138" s="65" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AK138" s="83"/>
-      <c r="AL138" s="112"/>
-      <c r="AM138" s="112"/>
-      <c r="AN138" s="112"/>
-      <c r="AO138" s="112"/>
-      <c r="AP138" s="112"/>
+      <c r="AL138" s="113"/>
+      <c r="AM138" s="113"/>
+      <c r="AN138" s="113"/>
+      <c r="AO138" s="113"/>
+      <c r="AP138" s="113"/>
     </row>
     <row r="139" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="108" t="n">
+      <c r="A139" s="109" t="n">
         <v>4212</v>
       </c>
       <c r="B139" s="84" t="n">
@@ -12418,10 +12429,10 @@
         <v>-1.81853514790593</v>
       </c>
       <c r="AF139" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG139" s="63" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AH139" s="64" t="n">
         <v>3</v>
@@ -12430,17 +12441,17 @@
         <v>44</v>
       </c>
       <c r="AJ139" s="65" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AK139" s="83"/>
-      <c r="AL139" s="112"/>
-      <c r="AM139" s="112"/>
-      <c r="AN139" s="112"/>
-      <c r="AO139" s="112"/>
-      <c r="AP139" s="112"/>
+      <c r="AL139" s="113"/>
+      <c r="AM139" s="113"/>
+      <c r="AN139" s="113"/>
+      <c r="AO139" s="113"/>
+      <c r="AP139" s="113"/>
     </row>
     <row r="140" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="123" t="n">
+      <c r="A140" s="124" t="n">
         <v>4212</v>
       </c>
       <c r="B140" s="86" t="n">
@@ -12504,29 +12515,29 @@
         <v>-0.741540402208021</v>
       </c>
       <c r="AF140" s="70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AG140" s="71" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AH140" s="72" t="n">
         <v>3</v>
       </c>
       <c r="AI140" s="72" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="AJ140" s="73" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AK140" s="83"/>
-      <c r="AL140" s="112"/>
-      <c r="AM140" s="112"/>
-      <c r="AN140" s="112"/>
-      <c r="AO140" s="112"/>
-      <c r="AP140" s="112"/>
+      <c r="AL140" s="113"/>
+      <c r="AM140" s="113"/>
+      <c r="AN140" s="113"/>
+      <c r="AO140" s="113"/>
+      <c r="AP140" s="113"/>
     </row>
     <row r="141" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="111" t="n">
+      <c r="A141" s="112" t="n">
         <f aca="false">A98+1000</f>
         <v>4213</v>
       </c>
@@ -12590,14 +12601,14 @@
       <c r="AI141" s="42"/>
       <c r="AJ141" s="73"/>
       <c r="AK141" s="35"/>
-      <c r="AL141" s="112"/>
-      <c r="AM141" s="112"/>
-      <c r="AN141" s="112"/>
-      <c r="AO141" s="112"/>
-      <c r="AP141" s="112"/>
+      <c r="AL141" s="113"/>
+      <c r="AM141" s="113"/>
+      <c r="AN141" s="113"/>
+      <c r="AO141" s="113"/>
+      <c r="AP141" s="113"/>
     </row>
     <row r="142" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="113" t="n">
+      <c r="A142" s="114" t="n">
         <f aca="false">A99+1000</f>
         <v>4221</v>
       </c>
@@ -12661,14 +12672,14 @@
       <c r="AI142" s="42"/>
       <c r="AJ142" s="27"/>
       <c r="AK142" s="35"/>
-      <c r="AL142" s="112"/>
-      <c r="AM142" s="112"/>
-      <c r="AN142" s="112"/>
-      <c r="AO142" s="112"/>
-      <c r="AP142" s="112"/>
+      <c r="AL142" s="113"/>
+      <c r="AM142" s="113"/>
+      <c r="AN142" s="113"/>
+      <c r="AO142" s="113"/>
+      <c r="AP142" s="113"/>
     </row>
     <row r="143" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="113" t="n">
+      <c r="A143" s="114" t="n">
         <f aca="false">A100+1000</f>
         <v>4222</v>
       </c>
@@ -12732,14 +12743,14 @@
       <c r="AI143" s="42"/>
       <c r="AJ143" s="27"/>
       <c r="AK143" s="35"/>
-      <c r="AL143" s="112"/>
-      <c r="AM143" s="112"/>
-      <c r="AN143" s="112"/>
-      <c r="AO143" s="112"/>
-      <c r="AP143" s="112"/>
+      <c r="AL143" s="113"/>
+      <c r="AM143" s="113"/>
+      <c r="AN143" s="113"/>
+      <c r="AO143" s="113"/>
+      <c r="AP143" s="113"/>
     </row>
     <row r="144" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="113" t="n">
+      <c r="A144" s="114" t="n">
         <f aca="false">A101+1000</f>
         <v>4223</v>
       </c>
@@ -12803,14 +12814,14 @@
       <c r="AI144" s="42"/>
       <c r="AJ144" s="27"/>
       <c r="AK144" s="35"/>
-      <c r="AL144" s="112"/>
-      <c r="AM144" s="112"/>
-      <c r="AN144" s="112"/>
-      <c r="AO144" s="112"/>
-      <c r="AP144" s="112"/>
+      <c r="AL144" s="113"/>
+      <c r="AM144" s="113"/>
+      <c r="AN144" s="113"/>
+      <c r="AO144" s="113"/>
+      <c r="AP144" s="113"/>
     </row>
     <row r="145" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="107" t="n">
+      <c r="A145" s="108" t="n">
         <f aca="false">A102+1000</f>
         <v>4311</v>
       </c>
@@ -12874,14 +12885,14 @@
       <c r="AI145" s="42"/>
       <c r="AJ145" s="27"/>
       <c r="AK145" s="35"/>
-      <c r="AL145" s="112"/>
-      <c r="AM145" s="112"/>
-      <c r="AN145" s="112"/>
-      <c r="AO145" s="112"/>
-      <c r="AP145" s="112"/>
+      <c r="AL145" s="113"/>
+      <c r="AM145" s="113"/>
+      <c r="AN145" s="113"/>
+      <c r="AO145" s="113"/>
+      <c r="AP145" s="113"/>
     </row>
     <row r="146" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="107" t="n">
+      <c r="A146" s="108" t="n">
         <f aca="false">A103+1000</f>
         <v>4312</v>
       </c>
@@ -12951,26 +12962,26 @@
         <v>46</v>
       </c>
       <c r="AG146" s="55" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH146" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI146" s="64" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="AJ146" s="82" t="s">
         <v>60</v>
       </c>
       <c r="AK146" s="83"/>
-      <c r="AL146" s="112"/>
-      <c r="AM146" s="112"/>
-      <c r="AN146" s="112"/>
-      <c r="AO146" s="112"/>
-      <c r="AP146" s="112"/>
+      <c r="AL146" s="113"/>
+      <c r="AM146" s="113"/>
+      <c r="AN146" s="113"/>
+      <c r="AO146" s="113"/>
+      <c r="AP146" s="113"/>
     </row>
     <row r="147" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="109" t="n">
+      <c r="A147" s="110" t="n">
         <f aca="false">A104+1000</f>
         <v>4312</v>
       </c>
@@ -13040,26 +13051,26 @@
         <v>46</v>
       </c>
       <c r="AG147" s="63" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AH147" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI147" s="64" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="AJ147" s="65" t="s">
         <v>60</v>
       </c>
       <c r="AK147" s="83"/>
-      <c r="AL147" s="112"/>
-      <c r="AM147" s="112"/>
-      <c r="AN147" s="112"/>
-      <c r="AO147" s="112"/>
-      <c r="AP147" s="112"/>
+      <c r="AL147" s="113"/>
+      <c r="AM147" s="113"/>
+      <c r="AN147" s="113"/>
+      <c r="AO147" s="113"/>
+      <c r="AP147" s="113"/>
     </row>
     <row r="148" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="108" t="n">
+      <c r="A148" s="109" t="n">
         <v>4312</v>
       </c>
       <c r="B148" s="84" t="n">
@@ -13134,20 +13145,20 @@
         <v>2</v>
       </c>
       <c r="AI148" s="64" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="AJ148" s="65" t="s">
         <v>60</v>
       </c>
       <c r="AK148" s="83"/>
-      <c r="AL148" s="112"/>
-      <c r="AM148" s="112"/>
-      <c r="AN148" s="112"/>
-      <c r="AO148" s="112"/>
-      <c r="AP148" s="112"/>
+      <c r="AL148" s="113"/>
+      <c r="AM148" s="113"/>
+      <c r="AN148" s="113"/>
+      <c r="AO148" s="113"/>
+      <c r="AP148" s="113"/>
     </row>
     <row r="149" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="108" t="n">
+      <c r="A149" s="109" t="n">
         <v>4312</v>
       </c>
       <c r="B149" s="84" t="n">
@@ -13216,26 +13227,26 @@
         <v>54</v>
       </c>
       <c r="AG149" s="63" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AH149" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI149" s="64" t="s">
-        <v>186</v>
+        <v>85</v>
       </c>
       <c r="AJ149" s="65" t="s">
         <v>60</v>
       </c>
       <c r="AK149" s="83"/>
-      <c r="AL149" s="112"/>
-      <c r="AM149" s="112"/>
-      <c r="AN149" s="112"/>
-      <c r="AO149" s="112"/>
-      <c r="AP149" s="112"/>
+      <c r="AL149" s="113"/>
+      <c r="AM149" s="113"/>
+      <c r="AN149" s="113"/>
+      <c r="AO149" s="113"/>
+      <c r="AP149" s="113"/>
     </row>
     <row r="150" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="108" t="n">
+      <c r="A150" s="109" t="n">
         <v>4312</v>
       </c>
       <c r="B150" s="84" t="n">
@@ -13308,15 +13319,15 @@
         <v>3</v>
       </c>
       <c r="AI150" s="64" t="s">
-        <v>186</v>
+        <v>59</v>
       </c>
       <c r="AJ150" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK150" s="83"/>
     </row>
     <row r="151" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="108" t="n">
+      <c r="A151" s="109" t="n">
         <v>4312</v>
       </c>
       <c r="B151" s="84" t="n">
@@ -13385,13 +13396,13 @@
         <v>56</v>
       </c>
       <c r="AG151" s="63" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AH151" s="64" t="n">
         <v>3</v>
       </c>
       <c r="AI151" s="64" t="s">
-        <v>186</v>
+        <v>85</v>
       </c>
       <c r="AJ151" s="65" t="s">
         <v>188</v>
@@ -13399,7 +13410,7 @@
       <c r="AK151" s="83"/>
     </row>
     <row r="152" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="123" t="n">
+      <c r="A152" s="124" t="n">
         <v>4312</v>
       </c>
       <c r="B152" s="86" t="n">
@@ -13472,15 +13483,15 @@
         <v>5</v>
       </c>
       <c r="AI152" s="72" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="AJ152" s="73" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AK152" s="83"/>
     </row>
     <row r="153" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="111" t="n">
+      <c r="A153" s="112" t="n">
         <f aca="false">A106+1000</f>
         <v>4313</v>
       </c>
@@ -13546,7 +13557,7 @@
       <c r="AK153" s="35"/>
     </row>
     <row r="154" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="113" t="n">
+      <c r="A154" s="114" t="n">
         <f aca="false">A107+1000</f>
         <v>4321</v>
       </c>
@@ -13612,7 +13623,7 @@
       <c r="AK154" s="35"/>
     </row>
     <row r="155" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="113" t="n">
+      <c r="A155" s="114" t="n">
         <f aca="false">A108+1000</f>
         <v>4322</v>
       </c>
@@ -13678,7 +13689,7 @@
       <c r="AK155" s="35"/>
     </row>
     <row r="156" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="107" t="n">
+      <c r="A156" s="108" t="n">
         <f aca="false">A109+1000</f>
         <v>4323</v>
       </c>
@@ -13744,7 +13755,7 @@
       <c r="AK156" s="35"/>
     </row>
     <row r="157" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="107" t="n">
+      <c r="A157" s="108" t="n">
         <f aca="false">A110+1000</f>
         <v>4411</v>
       </c>
@@ -13826,7 +13837,7 @@
         <v>30</v>
       </c>
       <c r="AI157" s="64" t="s">
-        <v>186</v>
+        <v>59</v>
       </c>
       <c r="AJ157" s="82" t="s">
         <v>91</v>
@@ -13834,7 +13845,7 @@
       <c r="AK157" s="83"/>
     </row>
     <row r="158" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="108" t="n">
+      <c r="A158" s="109" t="n">
         <v>4411</v>
       </c>
       <c r="B158" s="84" t="n">
@@ -13899,13 +13910,13 @@
         <v>52</v>
       </c>
       <c r="AG158" s="63" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AH158" s="64" t="n">
         <v>120</v>
       </c>
       <c r="AI158" s="64" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="AJ158" s="65" t="s">
         <v>191</v>
@@ -13913,7 +13924,7 @@
       <c r="AK158" s="83"/>
     </row>
     <row r="159" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="108" t="n">
+      <c r="A159" s="109" t="n">
         <v>4411</v>
       </c>
       <c r="B159" s="84" t="n">
@@ -13986,7 +13997,7 @@
         <v>120</v>
       </c>
       <c r="AI159" s="64" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="AJ159" s="65" t="s">
         <v>193</v>
@@ -13994,7 +14005,7 @@
       <c r="AK159" s="83"/>
     </row>
     <row r="160" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="108" t="n">
+      <c r="A160" s="109" t="n">
         <v>4411</v>
       </c>
       <c r="B160" s="84" t="n">
@@ -14062,16 +14073,16 @@
         <v>0.639807971304707</v>
       </c>
       <c r="AF160" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG160" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH160" s="72" t="n">
         <v>2</v>
       </c>
       <c r="AI160" s="72" t="s">
-        <v>186</v>
+        <v>82</v>
       </c>
       <c r="AJ160" s="73" t="s">
         <v>86</v>
@@ -14079,7 +14090,7 @@
       <c r="AK160" s="83"/>
     </row>
     <row r="161" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="107" t="n">
+      <c r="A161" s="108" t="n">
         <f aca="false">A111+1000</f>
         <v>4412</v>
       </c>
@@ -14169,7 +14180,7 @@
       <c r="AK161" s="83"/>
     </row>
     <row r="162" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="109" t="n">
+      <c r="A162" s="110" t="n">
         <f aca="false">A113+1000</f>
         <v>4412</v>
       </c>
@@ -14237,7 +14248,7 @@
         <v>54</v>
       </c>
       <c r="AG162" s="63" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AH162" s="64" t="n">
         <v>3</v>
@@ -14251,7 +14262,7 @@
       <c r="AK162" s="83"/>
     </row>
     <row r="163" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="123" t="n">
+      <c r="A163" s="124" t="n">
         <v>4412</v>
       </c>
       <c r="B163" s="86" t="n">
@@ -14329,7 +14340,7 @@
         <v>-1.30927557020858</v>
       </c>
       <c r="AF163" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG163" s="71" t="s">
         <v>195</v>
@@ -14338,7 +14349,7 @@
         <v>2</v>
       </c>
       <c r="AI163" s="72" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="AJ163" s="73" t="s">
         <v>86</v>
@@ -14346,7 +14357,7 @@
       <c r="AK163" s="83"/>
     </row>
     <row r="164" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="111" t="n">
+      <c r="A164" s="112" t="n">
         <f aca="false">A114+1000</f>
         <v>4413</v>
       </c>
@@ -14412,7 +14423,7 @@
       <c r="AK164" s="35"/>
     </row>
     <row r="165" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="113" t="n">
+      <c r="A165" s="114" t="n">
         <f aca="false">A115+1000</f>
         <v>4421</v>
       </c>
@@ -14478,7 +14489,7 @@
       <c r="AK165" s="35"/>
     </row>
     <row r="166" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="113" t="n">
+      <c r="A166" s="114" t="n">
         <f aca="false">A116+1000</f>
         <v>4422</v>
       </c>
@@ -14544,7 +14555,7 @@
       <c r="AK166" s="35"/>
     </row>
     <row r="167" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="113" t="n">
+      <c r="A167" s="114" t="n">
         <f aca="false">A117+1000</f>
         <v>4423</v>
       </c>
@@ -14610,13 +14621,13 @@
       <c r="AK167" s="35"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B168" s="124"/>
+      <c r="B168" s="125"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="125" t="s">
+      <c r="A169" s="126" t="s">
         <v>196</v>
       </c>
-      <c r="B169" s="124" t="n">
+      <c r="B169" s="125" t="n">
         <f aca="false">COUNTIF(B3:M167,"&gt;0")+COUNTIF(B3:M167,"&lt;0")</f>
         <v>206</v>
       </c>
@@ -14625,7 +14636,7 @@
       <c r="A170" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B170" s="124" t="n">
+      <c r="B170" s="125" t="n">
         <f aca="false">COUNTIF(N4:W168,"&gt;0")+COUNTIF(N4:W168,"&lt;0")</f>
         <v>237</v>
       </c>
@@ -14634,7 +14645,7 @@
       <c r="A171" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B171" s="124" t="n">
+      <c r="B171" s="125" t="n">
         <f aca="false">B169+B170</f>
         <v>443</v>
       </c>

</xml_diff>